<commit_message>
Correcta Autoevaluacio Ivan Rubi
</commit_message>
<xml_diff>
--- a/FullAutoavaluacio_IvanRubi.xlsx
+++ b/FullAutoavaluacio_IvanRubi.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_4929B44DB2784CE48377D498FEFE30612999DCB3" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{F65FDD11-1EE5-4354-AAEE-254C7916D317}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -98,8 +97,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +136,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -158,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -186,6 +193,7 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,53 +473,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="47.42578125" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.3984375" customWidth="1"/>
+    <col min="3" max="3" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B7" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -519,12 +527,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="86.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B16" s="2"/>
       <c r="C16" s="8" t="s">
         <v>2</v>
@@ -557,7 +565,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="B17" s="2"/>
       <c r="C17" s="2">
         <v>0.2</v>
@@ -590,7 +598,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B18" s="3"/>
       <c r="C18" s="3">
         <f>C17*100%</f>
@@ -633,7 +641,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B19" s="5" t="s">
         <v>11</v>
       </c>
@@ -662,13 +670,13 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="C20">
         <f>C19*C17</f>
         <v>0.2</v>
@@ -703,28 +711,28 @@
       </c>
       <c r="K20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="L20">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B22" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C22">
         <f>SUM(C20:L20)</f>
-        <v>0.8500000000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+        <v>0.90000000000000024</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B27" s="2"/>
       <c r="C27" s="8" t="s">
         <v>2</v>
@@ -757,7 +765,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="B28" s="3"/>
       <c r="C28" s="2">
         <v>0.2</v>
@@ -790,7 +798,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C29" s="3">
         <f>C28*100%</f>
         <v>0.2</v>
@@ -832,7 +840,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B30" s="5" t="s">
         <v>11</v>
       </c>
@@ -867,7 +875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="C31">
         <f>C30*C28</f>
         <v>0.2</v>
@@ -909,7 +917,10 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="H32" s="11"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B33" s="4" t="s">
         <v>15</v>
       </c>
@@ -918,36 +929,36 @@
         <v>0.80000000000000016</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B35" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C35">
         <f>C33/C22</f>
-        <v>0.94117647058823528</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B37" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C37">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B39" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C39">
         <f>C37*C35</f>
-        <v>7.5294117647058822</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+        <v>6.2222222222222214</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B41" s="6" t="s">
         <v>16</v>
       </c>

</xml_diff>